<commit_message>
project ideas and react_basic layout is added
</commit_message>
<xml_diff>
--- a/ClassWorks/JS_API_Fetch.xlsx
+++ b/ClassWorks/JS_API_Fetch.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="120">
   <si>
     <t>#</t>
   </si>
@@ -309,6 +309,81 @@
   </si>
   <si>
     <t>Nobel Prize Docs</t>
+  </si>
+  <si>
+    <t>Harsha</t>
+  </si>
+  <si>
+    <t>Manashvini</t>
+  </si>
+  <si>
+    <t>Charan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yashaswini </t>
+  </si>
+  <si>
+    <t>Nilima</t>
+  </si>
+  <si>
+    <t>SriHari</t>
+  </si>
+  <si>
+    <t>Vineeth</t>
+  </si>
+  <si>
+    <t>Kushbu</t>
+  </si>
+  <si>
+    <t>Sathvika</t>
+  </si>
+  <si>
+    <t>Revanth</t>
+  </si>
+  <si>
+    <t>HariPriya</t>
+  </si>
+  <si>
+    <t>Sai Vamsi</t>
+  </si>
+  <si>
+    <t>Supriya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohith </t>
+  </si>
+  <si>
+    <t>Shraviya</t>
+  </si>
+  <si>
+    <t>Vivek</t>
+  </si>
+  <si>
+    <t>Sanmuk</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Thusar</t>
+  </si>
+  <si>
+    <t>Pranitha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhaskar </t>
+  </si>
+  <si>
+    <t>Keerthana</t>
+  </si>
+  <si>
+    <t>Poojitha</t>
+  </si>
+  <si>
+    <t>Ramaraju</t>
   </si>
 </sst>
 </file>
@@ -665,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,9 +753,10 @@
     <col min="3" max="3" width="46.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -697,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -713,8 +789,14 @@
       <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -730,8 +812,14 @@
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -747,8 +835,14 @@
       <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -764,8 +858,14 @@
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -781,8 +881,14 @@
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -798,8 +904,14 @@
       <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -815,8 +927,14 @@
       <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="4" t="s">
         <v>27</v>
@@ -830,8 +948,14 @@
       <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="6" t="s">
         <v>69</v>
@@ -845,8 +969,14 @@
       <c r="E10" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -862,8 +992,14 @@
       <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
         <v>42</v>
@@ -877,8 +1013,14 @@
       <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -894,8 +1036,14 @@
       <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -911,8 +1059,14 @@
       <c r="E14" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>11</v>
       </c>
@@ -928,8 +1082,14 @@
       <c r="E15" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>12</v>
       </c>
@@ -945,8 +1105,14 @@
       <c r="E16" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>13</v>
       </c>
@@ -962,8 +1128,14 @@
       <c r="E17" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -979,8 +1151,14 @@
       <c r="E18" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>15</v>
       </c>
@@ -996,8 +1174,14 @@
       <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>16</v>
       </c>
@@ -1013,8 +1197,14 @@
       <c r="E20" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>17</v>
       </c>
@@ -1030,8 +1220,14 @@
       <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>18</v>
       </c>
@@ -1047,8 +1243,14 @@
       <c r="E22" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>19</v>
       </c>
@@ -1064,8 +1266,14 @@
       <c r="E23" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>20</v>
       </c>
@@ -1081,8 +1289,14 @@
       <c r="E24" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>21</v>
       </c>
@@ -1098,8 +1312,14 @@
       <c r="E25" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>118</v>
+      </c>
+      <c r="H25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>22</v>
       </c>
@@ -1115,8 +1335,14 @@
       <c r="E26" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>23</v>
       </c>
@@ -1133,7 +1359,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>24</v>
       </c>
@@ -1150,7 +1376,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>25</v>
       </c>

</xml_diff>